<commit_message>
Resolve test issues with outdated import spreadsheets.
</commit_message>
<xml_diff>
--- a/tools/developer_tools/portal_testing/PythonSeleniumTest/data/Cable Design Import.xlsx
+++ b/tools/developer_tools/portal_testing/PythonSeleniumTest/data/Cable Design Import.xlsx
@@ -69,11 +69,47 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Numeric ID or name of CDB cable type catalog item. Name must be unique and prefixed with '#'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Name/tag of assigned inventory item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Specify true/false for item with assigned inventory. Leave blank otherwise.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">Alternate cable name. Embedded '#cdbid# tag will be replaced with the internal CDB identifier (integer).</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,19 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Numeric ID or name of CDB cable type catalog item. Name must be unique and prefixed with '#'.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -217,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -241,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -265,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -301,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -325,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -337,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -361,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -373,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -433,7 +457,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -445,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -457,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -486,7 +510,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t xml:space="preserve">Existing Item ID</t>
   </si>
@@ -497,6 +521,15 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigned Inventory Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Installed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alt Name</t>
   </si>
   <si>
@@ -525,9 +558,6 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
   </si>
   <si>
     <t xml:space="preserve">Endpoint1</t>
@@ -685,8 +715,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -707,16 +741,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL22"/>
+  <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y22" activeCellId="0" sqref="Y22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,529 +867,538 @@
       <c r="AL1" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y2" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>41</v>
+      <c r="Q2" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="O3" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y3" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL3" s="0" t="s">
-        <v>41</v>
+      <c r="Q3" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="O4" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL4" s="0" t="s">
-        <v>41</v>
+      <c r="Q4" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="O5" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y5" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL5" s="0" t="s">
-        <v>41</v>
+      <c r="Q5" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="O6" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y6" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL6" s="0" t="s">
-        <v>41</v>
+      <c r="Q6" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="O7" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y7" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL7" s="0" t="s">
-        <v>41</v>
+      <c r="Q7" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="O8" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y8" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL8" s="0" t="s">
-        <v>41</v>
+      <c r="Q8" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="O9" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y9" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI9" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK9" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL9" s="0" t="s">
-        <v>41</v>
+      <c r="Q9" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA9" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="O10" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y10" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ10" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK10" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL10" s="0" t="s">
-        <v>41</v>
+      <c r="Q10" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA10" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="G11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="O11" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y11" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL11" s="0" t="s">
-        <v>41</v>
+      <c r="Q11" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA11" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="G12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="O12" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y12" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL12" s="0" t="s">
-        <v>41</v>
+      <c r="Q12" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="G13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="O13" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y13" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL13" s="0" t="s">
-        <v>41</v>
+      <c r="Q13" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA13" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="G14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="O14" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y14" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI14" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL14" s="0" t="s">
-        <v>41</v>
+      <c r="Q14" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA14" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="G15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="O15" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y15" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL15" s="0" t="s">
-        <v>41</v>
+      <c r="Q15" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA15" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN15" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="G16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="O16" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y16" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI16" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK16" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL16" s="0" t="s">
-        <v>41</v>
+      <c r="Q16" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA16" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN16" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="G17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="O17" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y17" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI17" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL17" s="0" t="s">
-        <v>41</v>
+      <c r="Q17" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN17" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="G18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="O18" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y18" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI18" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ18" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK18" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL18" s="0" t="s">
-        <v>41</v>
+      <c r="Q18" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA18" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN18" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="G19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="O19" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y19" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK19" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL19" s="0" t="s">
-        <v>41</v>
+      <c r="Q19" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA19" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="G20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="O20" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y20" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI20" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK20" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL20" s="0" t="s">
-        <v>41</v>
+      <c r="Q20" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA20" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="G21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="O21" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="Y21" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AI21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK21" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL21" s="0" t="s">
-        <v>41</v>
+      <c r="Q21" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AA21" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN21" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Resolve new column for cable design import test.
</commit_message>
<xml_diff>
--- a/tools/developer_tools/portal_testing/PythonSeleniumTest/data/Cable Design Import.xlsx
+++ b/tools/developer_tools/portal_testing/PythonSeleniumTest/data/Cable Design Import.xlsx
@@ -213,11 +213,23 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Total length of the cable required, including routed and end lengths. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">Cable notes.</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -229,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -241,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -265,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -301,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -325,7 +337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -337,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -361,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -373,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -397,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -433,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -445,7 +457,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -457,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -481,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -493,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -510,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="45">
   <si>
     <t xml:space="preserve">Existing Item ID</t>
   </si>
@@ -551,12 +563,15 @@
     <t xml:space="preserve">Voltage</t>
   </si>
   <si>
-    <t xml:space="preserve">Routed Length</t>
+    <t xml:space="preserve">Routed Length (ft)</t>
   </si>
   <si>
     <t xml:space="preserve">Route</t>
   </si>
   <si>
+    <t xml:space="preserve">Total Required Cable Length (ft)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
@@ -575,7 +590,7 @@
     <t xml:space="preserve">Endpoint1 Route</t>
   </si>
   <si>
-    <t xml:space="preserve">Endpoint1 End Length</t>
+    <t xml:space="preserve">Endpoint1 End Length (ft)</t>
   </si>
   <si>
     <t xml:space="preserve">Endpoint1 Termination</t>
@@ -605,7 +620,7 @@
     <t xml:space="preserve">Endpoint2 Route</t>
   </si>
   <si>
-    <t xml:space="preserve">Endpoint2 End Length</t>
+    <t xml:space="preserve">Endpoint2 End Length (ft)</t>
   </si>
   <si>
     <t xml:space="preserve">Endpoint2 Termination</t>
@@ -651,7 +666,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -671,6 +686,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -720,7 +741,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -741,15 +762,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN22"/>
+  <dimension ref="A1:AO21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,6 +894,9 @@
       <c r="AN1" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="AO1" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="n">
@@ -881,14 +905,17 @@
       <c r="G2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q2" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>40</v>
+      <c r="N2" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>41</v>
@@ -898,6 +925,9 @@
       </c>
       <c r="AN2" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,14 +937,17 @@
       <c r="G3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q3" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA3" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>40</v>
+      <c r="N3" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>501</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL3" s="1" t="s">
         <v>41</v>
@@ -924,6 +957,9 @@
       </c>
       <c r="AN3" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,14 +969,17 @@
       <c r="G4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="Q4" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA4" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>40</v>
+      <c r="N4" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>502</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL4" s="1" t="s">
         <v>41</v>
@@ -950,6 +989,9 @@
       </c>
       <c r="AN4" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,14 +1001,17 @@
       <c r="G5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Q5" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA5" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>40</v>
+      <c r="N5" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>503</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL5" s="1" t="s">
         <v>41</v>
@@ -976,6 +1021,9 @@
       </c>
       <c r="AN5" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,14 +1033,17 @@
       <c r="G6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="Q6" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA6" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>40</v>
+      <c r="N6" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>504</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL6" s="1" t="s">
         <v>41</v>
@@ -1002,6 +1053,9 @@
       </c>
       <c r="AN6" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,14 +1065,17 @@
       <c r="G7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="Q7" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA7" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK7" s="1" t="s">
-        <v>40</v>
+      <c r="N7" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>505</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL7" s="1" t="s">
         <v>41</v>
@@ -1028,6 +1085,9 @@
       </c>
       <c r="AN7" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,14 +1097,17 @@
       <c r="G8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="Q8" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA8" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK8" s="1" t="s">
-        <v>40</v>
+      <c r="N8" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>506</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL8" s="1" t="s">
         <v>41</v>
@@ -1054,6 +1117,9 @@
       </c>
       <c r="AN8" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,14 +1129,17 @@
       <c r="G9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="Q9" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA9" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK9" s="1" t="s">
-        <v>40</v>
+      <c r="N9" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>507</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB9" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL9" s="1" t="s">
         <v>41</v>
@@ -1080,6 +1149,9 @@
       </c>
       <c r="AN9" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,14 +1161,17 @@
       <c r="G10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="Q10" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA10" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK10" s="1" t="s">
-        <v>40</v>
+      <c r="N10" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>508</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB10" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL10" s="1" t="s">
         <v>41</v>
@@ -1106,6 +1181,9 @@
       </c>
       <c r="AN10" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,14 +1193,17 @@
       <c r="G11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="Q11" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA11" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK11" s="1" t="s">
-        <v>40</v>
+      <c r="N11" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>509</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB11" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL11" s="1" t="s">
         <v>41</v>
@@ -1132,6 +1213,9 @@
       </c>
       <c r="AN11" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,14 +1225,17 @@
       <c r="G12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="Q12" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA12" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK12" s="1" t="s">
-        <v>40</v>
+      <c r="N12" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>510</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL12" s="1" t="s">
         <v>41</v>
@@ -1158,6 +1245,9 @@
       </c>
       <c r="AN12" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,14 +1257,17 @@
       <c r="G13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="Q13" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA13" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK13" s="1" t="s">
-        <v>40</v>
+      <c r="N13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>511</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB13" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL13" s="1" t="s">
         <v>41</v>
@@ -1184,6 +1277,9 @@
       </c>
       <c r="AN13" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO13" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,14 +1289,17 @@
       <c r="G14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="Q14" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA14" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK14" s="1" t="s">
-        <v>40</v>
+      <c r="N14" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB14" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL14" s="1" t="s">
         <v>41</v>
@@ -1210,6 +1309,9 @@
       </c>
       <c r="AN14" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,14 +1321,17 @@
       <c r="G15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="Q15" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA15" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK15" s="1" t="s">
-        <v>40</v>
+      <c r="N15" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>513</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB15" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL15" s="1" t="s">
         <v>41</v>
@@ -1236,6 +1341,9 @@
       </c>
       <c r="AN15" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO15" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,14 +1353,17 @@
       <c r="G16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="Q16" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA16" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK16" s="1" t="s">
-        <v>40</v>
+      <c r="N16" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>514</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL16" s="1" t="s">
         <v>41</v>
@@ -1262,6 +1373,9 @@
       </c>
       <c r="AN16" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO16" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,14 +1385,17 @@
       <c r="G17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="Q17" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA17" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK17" s="1" t="s">
-        <v>40</v>
+      <c r="N17" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>515</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB17" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL17" s="1" t="s">
         <v>41</v>
@@ -1288,6 +1405,9 @@
       </c>
       <c r="AN17" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO17" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,14 +1417,17 @@
       <c r="G18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="Q18" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA18" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK18" s="1" t="s">
-        <v>40</v>
+      <c r="N18" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <v>516</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB18" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL18" s="1" t="s">
         <v>41</v>
@@ -1314,6 +1437,9 @@
       </c>
       <c r="AN18" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO18" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,14 +1449,17 @@
       <c r="G19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="Q19" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA19" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK19" s="1" t="s">
-        <v>40</v>
+      <c r="N19" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <v>517</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL19" s="1" t="s">
         <v>41</v>
@@ -1340,6 +1469,9 @@
       </c>
       <c r="AN19" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1349,14 +1481,17 @@
       <c r="G20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="Q20" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA20" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK20" s="1" t="s">
-        <v>40</v>
+      <c r="N20" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>518</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB20" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL20" s="1" t="s">
         <v>41</v>
@@ -1366,6 +1501,9 @@
       </c>
       <c r="AN20" s="1" t="s">
         <v>43</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,14 +1513,17 @@
       <c r="G21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="Q21" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AA21" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="AK21" s="1" t="s">
-        <v>40</v>
+      <c r="N21" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>519</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="AB21" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="AL21" s="1" t="s">
         <v>41</v>
@@ -1393,12 +1534,10 @@
       <c r="AN21" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="AO21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>